<commit_message>
Finished header labelling of AGS budget. Then standardized the way we handle and name budget .csvs.
</commit_message>
<xml_diff>
--- a/FOIA SAR data/NATO AGS/AGS Budget Docs Data Draw.xlsx
+++ b/FOIA SAR data/NATO AGS/AGS Budget Docs Data Draw.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12180" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Program Overview" sheetId="3" r:id="rId1"/>
@@ -785,7 +785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1223,9 +1223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2227,10 +2225,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2355,10 +2353,7 @@
         <v>825.01499999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -2373,96 +2368,111 @@
       <c r="M7" s="8"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10" t="s">
+      <c r="B9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="C9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="I9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="J9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="K9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="10" t="s">
+      <c r="L9" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8">
+      <c r="B10" s="8">
         <v>240.23400000000001</v>
       </c>
-      <c r="D9" s="8">
+      <c r="C10" s="8">
         <v>120.18</v>
       </c>
-      <c r="E9" s="8">
+      <c r="D10" s="8">
         <v>244.51400000000001</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="8">
+      <c r="E10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="8">
         <v>244.51400000000001</v>
       </c>
-      <c r="H9" s="8">
+      <c r="G10" s="8">
         <v>369.01400000000001</v>
       </c>
-      <c r="I9" s="8">
+      <c r="H10" s="8">
         <v>328.899</v>
       </c>
-      <c r="J9" s="8">
+      <c r="I10" s="8">
         <v>307.45100000000002</v>
       </c>
-      <c r="K9" s="8">
+      <c r="J10" s="8">
         <v>325.46300000000002</v>
       </c>
-      <c r="L9" s="8">
+      <c r="K10" s="8">
         <v>356.428</v>
       </c>
-      <c r="M9" s="8">
+      <c r="L10" s="8">
         <v>4504.1589999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2473,8 +2483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2726,14 +2736,13 @@
       <c r="A15" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="10"/>
+      <c r="B15" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="C15" s="10" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="10" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2741,14 +2750,13 @@
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="4"/>
+      <c r="B16" s="4">
+        <v>120.18</v>
+      </c>
       <c r="C16" s="4">
-        <v>120.18</v>
+        <v>244.51400000000001</v>
       </c>
       <c r="D16" s="4">
-        <v>244.51400000000001</v>
-      </c>
-      <c r="E16" s="4">
         <v>316.14800000000002</v>
       </c>
     </row>

</xml_diff>